<commit_message>
Adding zone c violations to the control chart.
</commit_message>
<xml_diff>
--- a/examples/example_data_with_faults.xlsx
+++ b/examples/example_data_with_faults.xlsx
@@ -128,11 +128,11 @@
   </sheetPr>
   <dimension ref="A4:B104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
@@ -503,7 +503,7 @@
         <v>44</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>-0.54855123706447</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +543,7 @@
         <v>49</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>-0.734355600581598</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adding trend zone violations.
</commit_message>
<xml_diff>
--- a/examples/example_data_with_faults.xlsx
+++ b/examples/example_data_with_faults.xlsx
@@ -128,8 +128,8 @@
   </sheetPr>
   <dimension ref="A4:B104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -183,7 +183,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.430312399385278</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -191,7 +191,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>-2.15170807861928</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -199,7 +199,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>-0.233622357725075</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,7 +207,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>-2.77473426337442</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,7 +223,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>-4.92442514335875</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added zone mixture violations along with the ability to turn off some violation types.
</commit_message>
<xml_diff>
--- a/examples/example_data_with_faults.xlsx
+++ b/examples/example_data_with_faults.xlsx
@@ -128,8 +128,8 @@
   </sheetPr>
   <dimension ref="A4:B104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -255,7 +255,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>-1.97346641013488</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -271,7 +271,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>-0.345807714048309</v>
+        <v>-2.6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -279,7 +279,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1.06024711386006</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,7 +295,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>-0.0286147866785392</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,7 +303,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>-2.35293705781414</v>
+        <v>-2.7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +543,7 @@
         <v>49</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>0.73</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adding stratification violation to the data.
</commit_message>
<xml_diff>
--- a/examples/example_data_with_faults.xlsx
+++ b/examples/example_data_with_faults.xlsx
@@ -128,11 +128,11 @@
   </sheetPr>
   <dimension ref="A4:B104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
@@ -559,7 +559,7 @@
         <v>51</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>-3.89876166638892</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,7 +567,7 @@
         <v>52</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>4.02737541784593</v>
+        <v>2.02737541784593</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +599,7 @@
         <v>56</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2.43325867810903</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +607,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>-5.68081265074957</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +631,7 @@
         <v>60</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>4.59480465877859</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +647,7 @@
         <v>62</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>-4.6026784605974</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added data with intentional overcontrol fault.
</commit_message>
<xml_diff>
--- a/examples/example_data_with_faults.xlsx
+++ b/examples/example_data_with_faults.xlsx
@@ -126,10 +126,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:B104"/>
+  <dimension ref="A4:B122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -946,6 +946,150 @@
         <v>0.323957026168126</v>
       </c>
     </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>-2.88333003678403</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>2.53389756171697</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>-2.45399065399328</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>-7.85260295716882</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>2.44345098578806</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>-1.24246538667722</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>2.03668545972892</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>-0.363658423954536</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>3.16646918371305</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>-2.61257155538862</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>2.41028056501556</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>-2.88333003678403</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>2.53389756171697</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>-2.45399065399328</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>2.44345098578806</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>-1.24246538667722</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>2.03668545972892</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>-0.363658423954536</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>